<commit_message>
update Allen Brain Atlas bins
Changed Other bin to just be the individual cell types
</commit_message>
<xml_diff>
--- a/Human/HumanAdult_CellTypes.xlsx
+++ b/Human/HumanAdult_CellTypes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\freya\NAS\mgriswold\CellProfileLibrary\Human\Adult\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\freya\NAS\mgriswold\CellProfileLibrary\Human\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3753BF22-CF99-428A-8C26-E11F9D474B98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900C6DD0-B954-4C6E-B09E-0E985D39EABD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13725" yWindow="810" windowWidth="7500" windowHeight="12300" firstSheet="6" activeTab="6" xr2:uid="{5C9D2128-D458-4151-9FDA-9AE92928DC2C}"/>
+    <workbookView xWindow="24990" yWindow="5445" windowWidth="7500" windowHeight="12300" xr2:uid="{5C9D2128-D458-4151-9FDA-9AE92928DC2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Brain_AllenBrainAtlas" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <sheet name="Spleen_HCA" sheetId="18" r:id="rId18"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Brain_AllenBrainAtlas!$B$2:$C$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">ImmuneTumor_safeTME!$B$2:$C$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="482">
   <si>
     <t>Main Cell Types</t>
   </si>
@@ -110,9 +111,6 @@
   </si>
   <si>
     <t>L6b</t>
-  </si>
-  <si>
-    <t>Other</t>
   </si>
   <si>
     <t>Astrocyte</t>
@@ -1945,19 +1943,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{975D7259-6A34-406F-9B31-9502DEA8F5D5}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1976,31 +1974,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2008,107 +2006,148 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B2:C2" xr:uid="{07550D59-7A16-4EB1-91C6-DF16B15E27C9}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C21">
+      <sortCondition ref="B2"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2128,7 +2167,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2147,10 +2186,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2158,10 +2197,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C4" t="s">
         <v>281</v>
-      </c>
-      <c r="C4" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2169,10 +2208,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C5" t="s">
         <v>283</v>
-      </c>
-      <c r="C5" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2180,10 +2219,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C6" t="s">
         <v>285</v>
-      </c>
-      <c r="C6" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2191,10 +2230,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2202,10 +2241,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2213,10 +2252,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" t="s">
         <v>289</v>
-      </c>
-      <c r="C9" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2224,10 +2263,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2235,10 +2274,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2246,20 +2285,20 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>291</v>
+      </c>
+      <c r="C12" t="s">
         <v>292</v>
-      </c>
-      <c r="C12" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2267,10 +2306,10 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2278,10 +2317,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2289,10 +2328,10 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2300,10 +2339,10 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
+        <v>298</v>
+      </c>
+      <c r="C18" t="s">
         <v>299</v>
-      </c>
-      <c r="C18" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2311,10 +2350,10 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2322,10 +2361,10 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C20" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2333,10 +2372,10 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2344,10 +2383,10 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2355,10 +2394,10 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
+        <v>304</v>
+      </c>
+      <c r="C23" t="s">
         <v>305</v>
-      </c>
-      <c r="C23" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2366,10 +2405,10 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2377,15 +2416,15 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
+        <v>307</v>
+      </c>
+      <c r="C25" t="s">
         <v>308</v>
-      </c>
-      <c r="C25" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2393,10 +2432,10 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
+        <v>310</v>
+      </c>
+      <c r="C27" t="s">
         <v>311</v>
-      </c>
-      <c r="C27" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2404,10 +2443,10 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2415,10 +2454,10 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
+        <v>313</v>
+      </c>
+      <c r="C29" t="s">
         <v>314</v>
-      </c>
-      <c r="C29" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2426,25 +2465,25 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
+        <v>315</v>
+      </c>
+      <c r="C30" t="s">
         <v>316</v>
-      </c>
-      <c r="C30" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2452,10 +2491,10 @@
         <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C34" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2463,10 +2502,10 @@
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C35" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -2489,7 +2528,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2508,10 +2547,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C3" t="s">
         <v>322</v>
-      </c>
-      <c r="C3" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2519,10 +2558,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2530,10 +2569,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C5" t="s">
         <v>325</v>
-      </c>
-      <c r="C5" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2541,10 +2580,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>326</v>
+      </c>
+      <c r="C6" t="s">
         <v>327</v>
-      </c>
-      <c r="C6" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2552,10 +2591,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C7" t="s">
         <v>329</v>
-      </c>
-      <c r="C7" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2563,15 +2602,15 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C8" t="s">
         <v>331</v>
-      </c>
-      <c r="C8" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2579,35 +2618,35 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
+        <v>333</v>
+      </c>
+      <c r="C10" t="s">
         <v>334</v>
-      </c>
-      <c r="C10" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2615,10 +2654,10 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
+        <v>340</v>
+      </c>
+      <c r="C16" t="s">
         <v>341</v>
-      </c>
-      <c r="C16" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2626,10 +2665,10 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
+        <v>342</v>
+      </c>
+      <c r="C17" t="s">
         <v>343</v>
-      </c>
-      <c r="C17" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2637,10 +2676,10 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
+        <v>344</v>
+      </c>
+      <c r="C18" t="s">
         <v>345</v>
-      </c>
-      <c r="C18" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2648,10 +2687,10 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2659,10 +2698,10 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
+        <v>347</v>
+      </c>
+      <c r="C20" t="s">
         <v>348</v>
-      </c>
-      <c r="C20" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2670,10 +2709,10 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
+        <v>349</v>
+      </c>
+      <c r="C21" t="s">
         <v>350</v>
-      </c>
-      <c r="C21" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2681,10 +2720,10 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
+        <v>351</v>
+      </c>
+      <c r="C22" t="s">
         <v>352</v>
-      </c>
-      <c r="C22" t="s">
-        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -2708,7 +2747,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2727,10 +2766,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2738,10 +2777,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
         <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2749,10 +2788,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s">
         <v>106</v>
-      </c>
-      <c r="C5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2760,10 +2799,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>371</v>
+      </c>
+      <c r="C6" t="s">
         <v>372</v>
-      </c>
-      <c r="C6" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2771,10 +2810,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>356</v>
+      </c>
+      <c r="C7" t="s">
         <v>357</v>
-      </c>
-      <c r="C7" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2782,20 +2821,20 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2803,10 +2842,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2814,10 +2853,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" t="s">
         <v>92</v>
-      </c>
-      <c r="C12" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2825,15 +2864,15 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2841,10 +2880,10 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s">
         <v>94</v>
-      </c>
-      <c r="C15" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2852,10 +2891,10 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2863,10 +2902,10 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
+        <v>363</v>
+      </c>
+      <c r="C17" t="s">
         <v>364</v>
-      </c>
-      <c r="C17" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2874,10 +2913,10 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2885,10 +2924,10 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2896,10 +2935,10 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
+        <v>226</v>
+      </c>
+      <c r="C20" t="s">
         <v>227</v>
-      </c>
-      <c r="C20" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2907,15 +2946,15 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
+        <v>365</v>
+      </c>
+      <c r="C21" t="s">
         <v>366</v>
-      </c>
-      <c r="C21" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2923,10 +2962,10 @@
         <v>17</v>
       </c>
       <c r="B23" t="s">
+        <v>368</v>
+      </c>
+      <c r="C23" t="s">
         <v>369</v>
-      </c>
-      <c r="C23" t="s">
-        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -2949,7 +2988,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2968,10 +3007,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" t="s">
         <v>198</v>
-      </c>
-      <c r="C3" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2979,10 +3018,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2990,15 +3029,15 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3006,10 +3045,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3017,20 +3056,20 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3038,10 +3077,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>340</v>
+      </c>
+      <c r="C11" t="s">
         <v>341</v>
-      </c>
-      <c r="C11" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3049,10 +3088,10 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3060,10 +3099,10 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3071,15 +3110,15 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3087,10 +3126,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3098,10 +3137,10 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3109,10 +3148,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C18" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -3136,7 +3175,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3155,10 +3194,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C3" t="s">
         <v>393</v>
-      </c>
-      <c r="C3" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3166,10 +3205,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>394</v>
+      </c>
+      <c r="C4" t="s">
         <v>395</v>
-      </c>
-      <c r="C4" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3177,10 +3216,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>396</v>
+      </c>
+      <c r="C5" t="s">
         <v>397</v>
-      </c>
-      <c r="C5" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3188,10 +3227,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>398</v>
+      </c>
+      <c r="C6" t="s">
         <v>399</v>
-      </c>
-      <c r="C6" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3199,10 +3238,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C7" t="s">
         <v>401</v>
-      </c>
-      <c r="C7" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3210,10 +3249,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>402</v>
+      </c>
+      <c r="C8" t="s">
         <v>403</v>
-      </c>
-      <c r="C8" t="s">
-        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -3237,7 +3276,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3256,15 +3295,15 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3272,10 +3311,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
         <v>60</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3283,15 +3322,15 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3299,10 +3338,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3310,10 +3349,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3321,10 +3360,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C10" t="s">
         <v>409</v>
-      </c>
-      <c r="C10" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3332,15 +3371,15 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
         <v>68</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3348,10 +3387,10 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3359,10 +3398,10 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
+        <v>410</v>
+      </c>
+      <c r="C14" t="s">
         <v>411</v>
-      </c>
-      <c r="C14" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3370,10 +3409,10 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
         <v>80</v>
-      </c>
-      <c r="C15" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3397,7 +3436,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3416,10 +3455,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3427,10 +3466,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3438,10 +3477,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3449,25 +3488,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3475,10 +3514,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3486,10 +3525,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3497,20 +3536,20 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -3534,7 +3573,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3553,10 +3592,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3564,25 +3603,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3590,15 +3629,15 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3606,10 +3645,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3617,20 +3656,20 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
+        <v>441</v>
+      </c>
+      <c r="C11" t="s">
         <v>442</v>
-      </c>
-      <c r="C11" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3638,15 +3677,15 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3654,15 +3693,15 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3670,10 +3709,10 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3681,10 +3720,10 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C19" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -3708,7 +3747,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="2"/>
@@ -3727,16 +3766,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3744,16 +3783,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3761,10 +3800,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3772,10 +3811,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C8" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3783,22 +3822,22 @@
         <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3806,22 +3845,22 @@
         <v>6</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
       <c r="C13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
       <c r="C14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3829,10 +3868,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="C15" t="s">
         <v>462</v>
-      </c>
-      <c r="C15" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3840,10 +3879,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C16" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3851,10 +3890,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3862,10 +3901,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="C18" t="s">
         <v>465</v>
-      </c>
-      <c r="C18" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3873,10 +3912,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="C19" t="s">
         <v>467</v>
-      </c>
-      <c r="C19" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3884,10 +3923,10 @@
         <v>12</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3895,10 +3934,10 @@
         <v>13</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3906,10 +3945,10 @@
         <v>14</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3917,16 +3956,16 @@
         <v>15</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
       <c r="C24" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -3934,10 +3973,10 @@
         <v>16</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C25" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3945,10 +3984,10 @@
         <v>17</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C26" t="s">
         <v>227</v>
-      </c>
-      <c r="C26" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3956,10 +3995,10 @@
         <v>18</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C27" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -3983,7 +4022,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4002,7 +4041,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -4033,7 +4072,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -4074,40 +4113,40 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -4131,7 +4170,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4150,15 +4189,15 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4166,10 +4205,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
         <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4177,10 +4216,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4188,10 +4227,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
         <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4199,10 +4238,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
         <v>40</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4210,30 +4249,30 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
         <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -4257,7 +4296,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4276,10 +4315,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" t="s">
         <v>114</v>
-      </c>
-      <c r="C3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4287,10 +4326,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
         <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4298,15 +4337,15 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
         <v>51</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4314,20 +4353,20 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
         <v>54</v>
-      </c>
-      <c r="C7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -4335,15 +4374,15 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4351,10 +4390,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
         <v>60</v>
-      </c>
-      <c r="C12" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -4362,15 +4401,15 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
         <v>62</v>
-      </c>
-      <c r="C13" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -4378,10 +4417,10 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -4389,10 +4428,10 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
         <v>66</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4400,20 +4439,20 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
         <v>68</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -4421,25 +4460,25 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="s">
         <v>72</v>
-      </c>
-      <c r="C20" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -4447,10 +4486,10 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -4458,10 +4497,10 @@
         <v>13</v>
       </c>
       <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
         <v>78</v>
-      </c>
-      <c r="C25" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -4469,10 +4508,10 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
         <v>80</v>
-      </c>
-      <c r="C26" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -4496,7 +4535,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4515,10 +4554,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
         <v>83</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4526,10 +4565,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" t="s">
         <v>112</v>
-      </c>
-      <c r="C4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4537,10 +4576,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
         <v>104</v>
-      </c>
-      <c r="C5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4548,10 +4587,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" t="s">
         <v>106</v>
-      </c>
-      <c r="C6" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4559,10 +4598,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
         <v>108</v>
-      </c>
-      <c r="C7" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4570,10 +4609,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
         <v>85</v>
-      </c>
-      <c r="C8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4581,25 +4620,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
         <v>87</v>
-      </c>
-      <c r="C9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -4607,10 +4646,10 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
         <v>92</v>
-      </c>
-      <c r="C13" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -4618,10 +4657,10 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" t="s">
         <v>94</v>
-      </c>
-      <c r="C14" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -4629,10 +4668,10 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -4640,10 +4679,10 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" t="s">
         <v>110</v>
-      </c>
-      <c r="C16" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4651,10 +4690,10 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s">
         <v>97</v>
-      </c>
-      <c r="C17" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -4662,10 +4701,10 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" t="s">
         <v>99</v>
-      </c>
-      <c r="C18" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -4673,10 +4712,10 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" t="s">
         <v>101</v>
-      </c>
-      <c r="C19" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -4700,7 +4739,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="2"/>
@@ -4719,82 +4758,82 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
         <v>116</v>
-      </c>
-      <c r="C3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="C11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
       <c r="C15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -4802,46 +4841,46 @@
         <v>2</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -4849,88 +4888,88 @@
         <v>3</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
       <c r="C31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="C35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -4938,64 +4977,64 @@
         <v>4</v>
       </c>
       <c r="B37" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" t="s">
         <v>147</v>
-      </c>
-      <c r="C37" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
       <c r="C39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
       <c r="C40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
       <c r="C41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
       <c r="C42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
       <c r="C43" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
       <c r="C44" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
       <c r="C45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="7"/>
       <c r="C46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -5003,76 +5042,76 @@
         <v>5</v>
       </c>
       <c r="B47" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C47" t="s">
         <v>157</v>
-      </c>
-      <c r="C47" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
       <c r="C48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
       <c r="C49" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
       <c r="C50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="7"/>
       <c r="C51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
       <c r="C52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" s="7"/>
       <c r="C53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
       <c r="C54" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" s="7"/>
       <c r="C55" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
       <c r="C56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57" s="7"/>
       <c r="C57" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
       <c r="C58" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -5080,40 +5119,40 @@
         <v>6</v>
       </c>
       <c r="B59" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C59" t="s">
         <v>166</v>
-      </c>
-      <c r="C59" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
       <c r="C60" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
       <c r="C61" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" s="7"/>
       <c r="C62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
       <c r="C63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64" s="7"/>
       <c r="C64" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -5121,22 +5160,22 @@
         <v>7</v>
       </c>
       <c r="B65" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C65" t="s">
         <v>173</v>
-      </c>
-      <c r="C65" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66" s="7"/>
       <c r="C66" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67" s="7"/>
       <c r="C67" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -5144,10 +5183,10 @@
         <v>8</v>
       </c>
       <c r="B68" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C68" t="s">
         <v>177</v>
-      </c>
-      <c r="C68" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -5155,148 +5194,148 @@
         <v>9</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B70" s="7"/>
       <c r="C70" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B71" s="7"/>
       <c r="C71" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B72" s="7"/>
       <c r="C72" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B73" s="7"/>
       <c r="C73" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B74" s="7"/>
       <c r="C74" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B75" s="7"/>
       <c r="C75" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B76" s="7"/>
       <c r="C76" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B77" s="7"/>
       <c r="C77" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B78" s="7"/>
       <c r="C78" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B79" s="7"/>
       <c r="C79" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B80" s="7"/>
       <c r="C80" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="7"/>
       <c r="C81" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="7"/>
       <c r="C82" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="7"/>
       <c r="C83" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="7"/>
       <c r="C84" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="7"/>
       <c r="C85" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" s="7"/>
       <c r="C86" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="7"/>
       <c r="C87" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="7"/>
       <c r="C88" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="7"/>
       <c r="C89" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="7"/>
       <c r="C90" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="7"/>
       <c r="C91" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="7"/>
       <c r="C92" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -5308,7 +5347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A379498-E7DC-4294-8E3E-84CB01EAD92A}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -5320,7 +5359,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="2"/>
@@ -5339,10 +5378,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" t="s">
         <v>198</v>
-      </c>
-      <c r="C3" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5350,15 +5389,15 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" t="s">
         <v>200</v>
-      </c>
-      <c r="C4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5366,10 +5405,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5377,10 +5416,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5388,10 +5427,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5399,10 +5438,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5410,10 +5449,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5421,10 +5460,10 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5432,10 +5471,10 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5443,10 +5482,10 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>206</v>
+      </c>
+      <c r="C13" t="s">
         <v>207</v>
-      </c>
-      <c r="C13" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -5468,7 +5507,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -5487,15 +5526,15 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" t="s">
         <v>249</v>
-      </c>
-      <c r="C3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5503,10 +5542,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5514,10 +5553,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6" t="s">
         <v>253</v>
-      </c>
-      <c r="C6" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5525,10 +5564,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
         <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5536,15 +5575,15 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" t="s">
         <v>211</v>
-      </c>
-      <c r="C8" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5552,15 +5591,15 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" t="s">
         <v>214</v>
-      </c>
-      <c r="C10" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5568,10 +5607,10 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>216</v>
+      </c>
+      <c r="C12" t="s">
         <v>217</v>
-      </c>
-      <c r="C12" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5579,10 +5618,10 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5590,10 +5629,10 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C14" t="s">
         <v>220</v>
-      </c>
-      <c r="C14" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -5601,10 +5640,10 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15" t="s">
         <v>222</v>
-      </c>
-      <c r="C15" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -5612,10 +5651,10 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C16" t="s">
         <v>224</v>
-      </c>
-      <c r="C16" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5623,10 +5662,10 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
+        <v>254</v>
+      </c>
+      <c r="C17" t="s">
         <v>255</v>
-      </c>
-      <c r="C17" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -5634,10 +5673,10 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5645,10 +5684,10 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5656,10 +5695,10 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
+        <v>226</v>
+      </c>
+      <c r="C20" t="s">
         <v>227</v>
-      </c>
-      <c r="C20" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -5667,10 +5706,10 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" t="s">
         <v>229</v>
-      </c>
-      <c r="C21" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -5678,10 +5717,10 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
+        <v>230</v>
+      </c>
+      <c r="C22" t="s">
         <v>231</v>
-      </c>
-      <c r="C22" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5689,10 +5728,10 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" t="s">
         <v>233</v>
-      </c>
-      <c r="C23" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -5717,7 +5756,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -5736,15 +5775,15 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5752,15 +5791,15 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5768,15 +5807,15 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5784,10 +5823,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5795,10 +5834,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5806,10 +5845,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5817,10 +5856,10 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5828,10 +5867,10 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5839,15 +5878,15 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -5855,10 +5894,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5866,10 +5905,10 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -5877,10 +5916,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5888,10 +5927,10 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5899,10 +5938,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add simplified brain & immune and HCA/HPA datasets
</commit_message>
<xml_diff>
--- a/Human/HumanAdult_CellTypes.xlsx
+++ b/Human/HumanAdult_CellTypes.xlsx
@@ -8,33 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\freya\NAS\mgriswold\CellProfileLibrary\Human\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900C6DD0-B954-4C6E-B09E-0E985D39EABD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88820C83-4F37-445B-B2AA-DD6A40D03580}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24990" yWindow="5445" windowWidth="7500" windowHeight="12300" xr2:uid="{5C9D2128-D458-4151-9FDA-9AE92928DC2C}"/>
+    <workbookView xWindow="-16320" yWindow="-7080" windowWidth="16440" windowHeight="28440" activeTab="2" xr2:uid="{5C9D2128-D458-4151-9FDA-9AE92928DC2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Brain_AllenBrainAtlas" sheetId="1" r:id="rId1"/>
     <sheet name="Brain_AllenBrainAtlas_Class" sheetId="2" r:id="rId2"/>
-    <sheet name="Colon_HCA" sheetId="3" r:id="rId3"/>
-    <sheet name="Decidua_HCA" sheetId="4" r:id="rId4"/>
-    <sheet name="Esophagus_HCA" sheetId="5" r:id="rId5"/>
-    <sheet name="Gut_HCA" sheetId="6" r:id="rId6"/>
-    <sheet name="Heart_HCA" sheetId="7" r:id="rId7"/>
-    <sheet name="ImmuneCensus_HCA" sheetId="8" r:id="rId8"/>
-    <sheet name="ImmuneTumor_safeTME" sheetId="9" r:id="rId9"/>
-    <sheet name="Kidney_HCA" sheetId="10" r:id="rId10"/>
-    <sheet name="Liver_HCA" sheetId="11" r:id="rId11"/>
-    <sheet name="Lung_HCA" sheetId="12" r:id="rId12"/>
-    <sheet name="Muscle_HCA" sheetId="13" r:id="rId13"/>
-    <sheet name="Pancreas_HCA" sheetId="14" r:id="rId14"/>
-    <sheet name="Placenta_HCA" sheetId="15" r:id="rId15"/>
-    <sheet name="Retina_HCA" sheetId="16" r:id="rId16"/>
-    <sheet name="Skin_HCA" sheetId="17" r:id="rId17"/>
-    <sheet name="Spleen_HCA" sheetId="18" r:id="rId18"/>
+    <sheet name="Brain_Darmanis" sheetId="21" r:id="rId3"/>
+    <sheet name="Colon_HCA" sheetId="3" r:id="rId4"/>
+    <sheet name="Decidua_HCA" sheetId="4" r:id="rId5"/>
+    <sheet name="Esophagus_HCA" sheetId="5" r:id="rId6"/>
+    <sheet name="Gut_HCA" sheetId="6" r:id="rId7"/>
+    <sheet name="Heart_HCA" sheetId="7" r:id="rId8"/>
+    <sheet name="Ileum_Wang" sheetId="19" r:id="rId9"/>
+    <sheet name="ImmuneCensus_HCA" sheetId="8" r:id="rId10"/>
+    <sheet name="ImmuneTumor_safeTME" sheetId="9" r:id="rId11"/>
+    <sheet name="Kidney_HCA" sheetId="10" r:id="rId12"/>
+    <sheet name="Liver_HCA" sheetId="11" r:id="rId13"/>
+    <sheet name="Lung_HCA" sheetId="12" r:id="rId14"/>
+    <sheet name="Muscle_HCA" sheetId="13" r:id="rId15"/>
+    <sheet name="Pancreas_HCA" sheetId="14" r:id="rId16"/>
+    <sheet name="Placenta_HCA" sheetId="15" r:id="rId17"/>
+    <sheet name="Rectum_Wang" sheetId="20" r:id="rId18"/>
+    <sheet name="Retina_HCA" sheetId="16" r:id="rId19"/>
+    <sheet name="Skin_HCA" sheetId="17" r:id="rId20"/>
+    <sheet name="Spleen_HCA" sheetId="18" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Brain_AllenBrainAtlas!$B$2:$C$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">ImmuneTumor_safeTME!$B$2:$C$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Brain_Darmanis!$B$2:$C$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Ileum_Wang!$B$2:$C$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">ImmuneTumor_safeTME!$B$2:$C$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="501">
   <si>
     <t>Main Cell Types</t>
   </si>
@@ -1500,6 +1505,63 @@
   </si>
   <si>
     <t>Spleen - HCA</t>
+  </si>
+  <si>
+    <t>Stem Cell</t>
+  </si>
+  <si>
+    <t>Progenitor</t>
+  </si>
+  <si>
+    <t>Paneth-like</t>
+  </si>
+  <si>
+    <t>Goblet</t>
+  </si>
+  <si>
+    <t>Enteriendocrine</t>
+  </si>
+  <si>
+    <t>Ileum Wang</t>
+  </si>
+  <si>
+    <t>Rectum Wang</t>
+  </si>
+  <si>
+    <t>Brain Darmanis</t>
+  </si>
+  <si>
+    <t>Myeloid Type 1</t>
+  </si>
+  <si>
+    <t>Myeloid Type 2</t>
+  </si>
+  <si>
+    <t>Neoplastic</t>
+  </si>
+  <si>
+    <t>Neoplastic Type 1</t>
+  </si>
+  <si>
+    <t>Neoplastic Type 2</t>
+  </si>
+  <si>
+    <t>Neoplastic Type 3</t>
+  </si>
+  <si>
+    <t>Neuron</t>
+  </si>
+  <si>
+    <t>Vascular</t>
+  </si>
+  <si>
+    <t>Vascular Type 1</t>
+  </si>
+  <si>
+    <t>Vascular Type 2</t>
+  </si>
+  <si>
+    <t>Vascular Type 3</t>
   </si>
 </sst>
 </file>
@@ -1943,7 +2005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{975D7259-6A34-406F-9B31-9502DEA8F5D5}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -2153,6 +2215,467 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0D9AA6-8D2A-4785-8A66-0F92DFA6F6FD}">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>216</v>
+      </c>
+      <c r="C12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C13" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C16" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>254</v>
+      </c>
+      <c r="C17" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>226</v>
+      </c>
+      <c r="C20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>230</v>
+      </c>
+      <c r="C22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A14DC9-1AED-4FF8-A738-FF1FA0ECC161}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>278</v>
+      </c>
+      <c r="C10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>276</v>
+      </c>
+      <c r="C14" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>277</v>
+      </c>
+      <c r="C16" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C17" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>193</v>
+      </c>
+      <c r="C20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B2:C2" xr:uid="{B56D667B-DA06-455E-A7C3-3A4D247AFF62}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C20">
+      <sortCondition ref="B2"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C82DADD8-B503-48E2-9D35-7F9DED6C5A1F}">
   <dimension ref="A1:C35"/>
   <sheetViews>
@@ -2513,7 +3036,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9162C64-83A9-488D-BFF5-1E74B1241652}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -2731,7 +3254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3DBAD6-4DDD-485C-863D-4DADEEC42C74}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -2973,7 +3496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA5C1D0-A54E-4EAD-90EA-A0E787426882}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -3159,7 +3682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD5A76E-AD40-47EA-B7D5-43CFA6316762}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -3260,7 +3783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C830E4D-5D34-4AD1-A73C-E97AAA240212}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -3420,7 +3943,118 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9150CF0F-B10B-4446-B409-1AC5722C64D7}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I72" sqref="I72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>486</v>
+      </c>
+      <c r="C3" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>485</v>
+      </c>
+      <c r="C5" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>484</v>
+      </c>
+      <c r="C6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>483</v>
+      </c>
+      <c r="C7" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>482</v>
+      </c>
+      <c r="C8" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39B70E5-DC6A-44F1-B910-3188BFDBC930}">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -3550,455 +4184,6 @@
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>431</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB01F430-6301-4DFC-9BDB-9D080B1DB95A}">
-  <dimension ref="A1:C19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>452</v>
-      </c>
-      <c r="C3" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C4" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>453</v>
-      </c>
-      <c r="C8" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>440</v>
-      </c>
-      <c r="C10" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>441</v>
-      </c>
-      <c r="C11" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>454</v>
-      </c>
-      <c r="C14" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>450</v>
-      </c>
-      <c r="C19" t="s">
-        <v>450</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBA6F04-9723-49BD-8D25-48AA0B163B9E}">
-  <dimension ref="A1:C27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B17:B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>457</v>
-      </c>
-      <c r="C5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>458</v>
-      </c>
-      <c r="C7" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>459</v>
-      </c>
-      <c r="C8" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>460</v>
-      </c>
-      <c r="C9" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>7</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>461</v>
-      </c>
-      <c r="C15" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>8</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>463</v>
-      </c>
-      <c r="C16" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>9</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="C17" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>10</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>464</v>
-      </c>
-      <c r="C18" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>11</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>466</v>
-      </c>
-      <c r="C19" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>12</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>13</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>14</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="C22" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>15</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="8"/>
-      <c r="C24" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>16</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>469</v>
-      </c>
-      <c r="C25" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>17</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="C26" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>18</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>470</v>
-      </c>
-      <c r="C27" t="s">
-        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -4154,7 +4339,599 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB01F430-6301-4DFC-9BDB-9D080B1DB95A}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C3" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>453</v>
+      </c>
+      <c r="C8" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>440</v>
+      </c>
+      <c r="C10" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>441</v>
+      </c>
+      <c r="C11" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>454</v>
+      </c>
+      <c r="C14" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>450</v>
+      </c>
+      <c r="C19" t="s">
+        <v>450</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBA6F04-9723-49BD-8D25-48AA0B163B9E}">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B17:B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="C7" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="C8" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="C9" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="C15" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="C16" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C17" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="C18" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="C19" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C22" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>16</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="C25" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>17</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C26" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>18</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="C27" t="s">
+        <v>470</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{591929B5-5275-46A5-B3C8-5698ABC70041}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>492</v>
+      </c>
+      <c r="C6" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>496</v>
+      </c>
+      <c r="C9" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>497</v>
+      </c>
+      <c r="C12" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B2:C122" xr:uid="{055D2D1D-9338-4BBD-A31C-D0F7D4429283}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C21">
+      <sortCondition ref="C2:C122"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5827B9F-ECC4-49ED-9787-429F600A1943}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -4280,7 +5057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF470166-6ED0-446F-8F56-53780AB77E32}">
   <dimension ref="A1:C26"/>
   <sheetViews>
@@ -4519,7 +5296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599F1995-F13D-4EC1-965C-6DCCFD915A08}">
   <dimension ref="A1:C19"/>
   <sheetViews>
@@ -4723,7 +5500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAFDFD3-B7AD-47F5-84D7-2FE212B59B7D}">
   <dimension ref="A1:C92"/>
   <sheetViews>
@@ -5343,7 +6120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A379498-E7DC-4294-8E3E-84CB01EAD92A}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -5493,21 +6270,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0D9AA6-8D2A-4785-8A66-0F92DFA6F6FD}">
-  <dimension ref="A1:C23"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7C676A-FA05-44AF-8FD5-90A58FB5088E}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>257</v>
+        <v>487</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -5526,428 +6306,82 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>486</v>
       </c>
       <c r="C3" t="s">
-        <v>249</v>
+        <v>486</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
       <c r="C4" t="s">
-        <v>250</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>251</v>
+        <v>485</v>
       </c>
       <c r="C5" t="s">
-        <v>251</v>
+        <v>485</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>252</v>
+        <v>484</v>
       </c>
       <c r="C6" t="s">
-        <v>253</v>
+        <v>484</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>483</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>483</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>482</v>
       </c>
       <c r="C8" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>216</v>
-      </c>
-      <c r="C12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>218</v>
-      </c>
-      <c r="C13" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>219</v>
-      </c>
-      <c r="C14" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>221</v>
-      </c>
-      <c r="C15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>223</v>
-      </c>
-      <c r="C16" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>254</v>
-      </c>
-      <c r="C17" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>15</v>
-      </c>
-      <c r="B20" t="s">
-        <v>226</v>
-      </c>
-      <c r="C20" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>16</v>
-      </c>
-      <c r="B21" t="s">
-        <v>228</v>
-      </c>
-      <c r="C21" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>17</v>
-      </c>
-      <c r="B22" t="s">
-        <v>230</v>
-      </c>
-      <c r="C22" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>18</v>
-      </c>
-      <c r="B23" t="s">
-        <v>232</v>
-      </c>
-      <c r="C23" t="s">
-        <v>233</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A14DC9-1AED-4FF8-A738-FF1FA0ECC161}">
-  <dimension ref="A1:C20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>273</v>
-      </c>
-      <c r="C5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>274</v>
-      </c>
-      <c r="C7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>264</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>144</v>
       </c>
       <c r="C9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>278</v>
-      </c>
-      <c r="C10" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>275</v>
-      </c>
-      <c r="C13" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>276</v>
-      </c>
-      <c r="C14" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>277</v>
-      </c>
-      <c r="C16" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>11</v>
-      </c>
-      <c r="B17" t="s">
-        <v>265</v>
-      </c>
-      <c r="C17" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>164</v>
-      </c>
-      <c r="C18" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>193</v>
-      </c>
-      <c r="C20" t="s">
-        <v>193</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:C2" xr:uid="{B56D667B-DA06-455E-A7C3-3A4D247AFF62}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C20">
-      <sortCondition ref="B2"/>
+  <autoFilter ref="B2:C122" xr:uid="{055D2D1D-9338-4BBD-A31C-D0F7D4429283}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C14">
+      <sortCondition ref="C2:C122"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>